<commit_message>
add new emip cover
</commit_message>
<xml_diff>
--- a/cv-data.xlsx
+++ b/cv-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/w449t405/Documents/GIT/websites/cv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF0B875-9065-F940-B737-BEB6A7BE40F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFB66EB-60A4-EB4F-8E99-D2077CC55C3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="13800" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="18780" windowHeight="17040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="77">
   <si>
     <t>in_resume</t>
   </si>
@@ -264,7 +264,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1105,11 +1105,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
@@ -1117,7 +1117,7 @@
     <col min="6" max="9" width="32.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="17">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="51">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="51">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1223,7 +1223,7 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.5" bestFit="1" customWidth="1"/>
@@ -1232,7 +1232,7 @@
     <col min="7" max="9" width="43.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="17">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="85">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="102">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1380,10 +1380,10 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.5" customWidth="1"/>
@@ -1393,7 +1393,7 @@
     <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="17">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="34">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -1433,16 +1433,16 @@
         <v>72</v>
       </c>
       <c r="E2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="F2">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G2" s="3">
         <v>225000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="51">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -1456,17 +1456,17 @@
         <v>72</v>
       </c>
       <c r="E3">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="F3">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="34">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="34">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -1503,10 +1503,10 @@
         <v>72</v>
       </c>
       <c r="E5">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F5">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="G5" s="3">
         <v>225000</v>
@@ -1531,19 +1531,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F508133-2F1C-F74C-9A6E-5E2385798E5D}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="60.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -1568,60 +1568,60 @@
         <v>43</v>
       </c>
       <c r="C2">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
         <v>43</v>
       </c>
       <c r="C3">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="C4">
-        <v>2014</v>
-      </c>
-      <c r="D4">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>2014</v>
       </c>
+      <c r="D5">
+        <v>2018</v>
+      </c>
       <c r="E5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
         <v>47</v>
@@ -1633,29 +1633,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C7">
-        <v>2010</v>
-      </c>
-      <c r="D7">
         <v>2014</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="C8">
         <v>2010</v>
@@ -1664,34 +1661,51 @@
         <v>2014</v>
       </c>
       <c r="E8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>2010</v>
       </c>
+      <c r="D9">
+        <v>2014</v>
+      </c>
       <c r="E9" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10">
+        <v>2010</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
         <v>54</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>2009</v>
       </c>
-      <c r="E10" t="b">
+      <c r="E11" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1708,32 +1722,32 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
update ismart for grant extension
</commit_message>
<xml_diff>
--- a/cv-data.xlsx
+++ b/cv-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/websites/cv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E65351-6DB9-3343-B75B-9821E791EEC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8879E07-D9D5-EA4C-BA4D-32353558D075}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="18780" windowHeight="17040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="75">
   <si>
     <t>in_resume</t>
   </si>
@@ -243,12 +243,6 @@
   </si>
   <si>
     <t>USED, Institute of Education Sciences</t>
-  </si>
-  <si>
-    <t>Paths to Success: The Relationship of Academic and Career Skills to Postsecondary Employment Outcomes for Students with Significant Cognitive Disabilities</t>
-  </si>
-  <si>
-    <t>Gail Tiemann</t>
   </si>
   <si>
     <t>description_4</t>
@@ -1143,7 +1137,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J1" t="s">
         <v>0</v>
@@ -1204,7 +1198,7 @@
         <v>17</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
@@ -1377,10 +1371,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B7310B-209B-5F48-96E7-648531B2B600}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1442,73 +1436,49 @@
         <v>225000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
         <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E3">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="F3">
-        <v>2025</v>
-      </c>
-      <c r="G3" s="3"/>
+        <v>2020</v>
+      </c>
       <c r="H3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E4">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="F4">
-        <v>2020</v>
-      </c>
-      <c r="H4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5">
-        <v>2020</v>
-      </c>
-      <c r="F5">
         <v>2022</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G4" s="3">
         <v>225000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add links to advisor websites
</commit_message>
<xml_diff>
--- a/cv-data.xlsx
+++ b/cv-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/websites/cv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9238B41F-A58C-2445-9214-0ABD4F6C41C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532D3EBD-1D27-7F42-81C8-0C20F07237B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="18780" windowHeight="17040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="18780" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="3" r:id="rId1"/>
@@ -107,9 +107,6 @@
     <t>2019-04</t>
   </si>
   <si>
-    <t>Advisor: Neal Kingston</t>
-  </si>
-  <si>
     <t>Develop internal and external R packages</t>
   </si>
   <si>
@@ -191,9 +188,6 @@
     <t>Kansas Honor's Scholar</t>
   </si>
   <si>
-    <t>Advisor: Evangelia G. Chrysikou</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
@@ -255,6 +249,12 @@
   </si>
   <si>
     <t>Data-driven, Accelerated Academic Recovery (DAAR) for Students with Significant Cognitive Disabilities</t>
+  </si>
+  <si>
+    <t>Advisor: [Neal Kingston, Ph.D.](https://nealkingston.ku.edu/)</t>
+  </si>
+  <si>
+    <t>Advisor: [Evangelia G. Chrysikou, Ph.D.](https://www.chrysikoulab.com/)</t>
   </si>
 </sst>
 </file>
@@ -1105,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1143,7 +1143,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J1" t="s">
         <v>0</v>
@@ -1169,7 +1169,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>14</v>
@@ -1198,13 +1198,13 @@
         <v>16</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
@@ -1281,13 +1281,13 @@
         <v>26</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1352,22 +1352,22 @@
     </row>
     <row r="6" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
         <v>31</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>32</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>33</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1379,7 +1379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B7310B-209B-5F48-96E7-648531B2B600}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1395,16 +1395,16 @@
   <sheetData>
     <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -1413,24 +1413,24 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E2">
         <v>2022</v>
@@ -1439,21 +1439,21 @@
         <v>2025</v>
       </c>
       <c r="H2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E3">
         <v>2021</v>
@@ -1467,16 +1467,16 @@
     </row>
     <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E4">
         <v>2016</v>
@@ -1485,21 +1485,21 @@
         <v>2020</v>
       </c>
       <c r="H4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E5">
         <v>2020</v>
@@ -1544,27 +1544,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>40</v>
-      </c>
-      <c r="E1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
       </c>
       <c r="C2">
         <v>2020</v>
@@ -1575,10 +1575,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
         <v>42</v>
-      </c>
-      <c r="B3" t="s">
-        <v>43</v>
       </c>
       <c r="C3">
         <v>2017</v>
@@ -1589,10 +1589,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4">
         <v>2016</v>
@@ -1603,7 +1603,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -1620,10 +1620,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
         <v>46</v>
-      </c>
-      <c r="B6" t="s">
-        <v>47</v>
       </c>
       <c r="C6">
         <v>2014</v>
@@ -1634,10 +1634,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7">
         <v>2014</v>
@@ -1648,10 +1648,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
         <v>49</v>
-      </c>
-      <c r="B8" t="s">
-        <v>50</v>
       </c>
       <c r="C8">
         <v>2010</v>
@@ -1665,7 +1665,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -1682,10 +1682,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
         <v>52</v>
-      </c>
-      <c r="B10" t="s">
-        <v>53</v>
       </c>
       <c r="C10">
         <v>2010</v>
@@ -1696,7 +1696,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -1728,27 +1728,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update DLM status to Co-PI
</commit_message>
<xml_diff>
--- a/cv-data.xlsx
+++ b/cv-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/websites/cv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D6015D-CBBB-2444-B3AD-8BDAC46D92F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2266342D-DC3A-334A-8396-BDFDF6308439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="18780" windowHeight="17040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="18780" windowHeight="17040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="82">
   <si>
     <t>in_resume</t>
   </si>
@@ -261,6 +261,15 @@
   </si>
   <si>
     <t>Member of  ATLAS psychometric team working across projects including [Dynamic Learning Maps](https://dynamiclearningmaps.org) and the R package [measr](https://measr.info)</t>
+  </si>
+  <si>
+    <t>Co-Principal Investigator</t>
+  </si>
+  <si>
+    <t>Dynamic Learning Maps Alternate Assessment System</t>
+  </si>
+  <si>
+    <t>Ongoing state contracts</t>
   </si>
 </sst>
 </file>
@@ -1225,7 +1234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -1403,10 +1412,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B7310B-209B-5F48-96E7-648531B2B600}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1445,72 +1454,89 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2">
-        <v>2021</v>
-      </c>
-      <c r="F2">
-        <v>2023</v>
-      </c>
-      <c r="G2" s="3">
-        <v>225000</v>
+        <v>81</v>
+      </c>
+      <c r="H2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E3">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="F3">
-        <v>2020</v>
-      </c>
-      <c r="H3" t="s">
-        <v>65</v>
+        <v>2023</v>
+      </c>
+      <c r="G3" s="3">
+        <v>225000</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4">
+        <v>2016</v>
+      </c>
+      <c r="F4">
+        <v>2020</v>
+      </c>
+      <c r="H4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>54</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>68</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>2020</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>2022</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G5" s="3">
         <v>225000</v>
       </c>
     </row>
@@ -1523,7 +1549,7 @@
           <x14:formula1>
             <xm:f>'data-validation'!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A1048576</xm:sqref>
+          <xm:sqref>A3:A1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
add dissertation links; add division h award
</commit_message>
<xml_diff>
--- a/cv-data.xlsx
+++ b/cv-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/websites/cv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA46BCE4-3DDD-CE4C-897B-931D883B051A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DEDA8B-69E8-AB47-870E-F11CA1215093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="26540" windowHeight="17040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="26540" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="84">
   <si>
     <t>in_resume</t>
   </si>
@@ -65,18 +65,12 @@
     <t>Lawrence, KS</t>
   </si>
   <si>
-    <t>Dissertation: "Evaluating Model Estimation Processes for Diagnostic Classification Models"</t>
-  </si>
-  <si>
     <t>Emphasis: Research, Evaluation, Measurement, and Statistics</t>
   </si>
   <si>
     <t>B.S., Behavioral Neuroscience</t>
   </si>
   <si>
-    <t>Honors Thesis: "Dissociating Cognitive and Affective Empathy in Unipolar Depression"</t>
-  </si>
-  <si>
     <t>Minor: Social and Behavioral Sciences Methodology</t>
   </si>
   <si>
@@ -263,9 +257,6 @@
     <t>Assistant Director of Psychometrics</t>
   </si>
   <si>
-    <t>Lead a team of 2–3 reports to execute operational scoring and reporting and for the [Dynamic Learning Maps](https://dynamiclearningmaps.org) Alternate Assessment</t>
-  </si>
-  <si>
     <t>Develop and lead the implementation of a psychometric research program focused on diagnostic classification modeling, including presentation of findings to a variety of audiences</t>
   </si>
   <si>
@@ -273,6 +264,18 @@
   </si>
   <si>
     <t>Work across contract and grant-funded projects to promote learning, evaluate student achievement, and develop tools to improve research practice</t>
+  </si>
+  <si>
+    <t>AERA Division H Outstanding Publication Winner</t>
+  </si>
+  <si>
+    <t>Lead a team of 3–4 reports to execute operational scoring and reporting and for the [Dynamic Learning Maps](https://dynamiclearningmaps.org) Alternate Assessment</t>
+  </si>
+  <si>
+    <t>Dissertation: "[Evaluating Model Estimation Processes for Diagnostic Classification Models](https://doi.org/10.31237/osf.io/vke5u)"</t>
+  </si>
+  <si>
+    <t>Honors Thesis: "[Dissociating Cognitive and Affective Empathy in Unipolar Depression](https://doi.org/10.31237/osf.io/m4xjf)"</t>
   </si>
 </sst>
 </file>
@@ -1123,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1161,13 +1164,13 @@
         <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1184,21 +1187,21 @@
         <v>2018</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="J2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -1213,16 +1216,16 @@
         <v>2014</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
@@ -1237,8 +1240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1255,7 +1258,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -1279,7 +1282,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K1" t="s">
         <v>0</v>
@@ -1287,10 +1290,10 @@
     </row>
     <row r="2" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -1299,27 +1302,27 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -1328,18 +1331,18 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -1348,18 +1351,18 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -1368,10 +1371,10 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -1379,7 +1382,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -1388,30 +1391,30 @@
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1439,16 +1442,16 @@
   <sheetData>
     <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -1457,41 +1460,41 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" t="s">
-        <v>77</v>
-      </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E3">
         <v>2021</v>
@@ -1505,16 +1508,16 @@
     </row>
     <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E4">
         <v>2016</v>
@@ -1523,21 +1526,21 @@
         <v>2020</v>
       </c>
       <c r="H4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E5">
         <v>2020</v>
@@ -1568,10 +1571,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F508133-2F1C-F74C-9A6E-5E2385798E5D}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1582,30 +1585,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>34</v>
-      </c>
-      <c r="D1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C2">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -1613,13 +1616,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="C3">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -1627,13 +1630,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -1641,13 +1644,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C5">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -1655,16 +1658,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C6">
-        <v>2014</v>
-      </c>
-      <c r="D6">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -1672,24 +1672,27 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>2014</v>
       </c>
+      <c r="D7">
+        <v>2018</v>
+      </c>
       <c r="E7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8">
         <v>2014</v>
@@ -1700,15 +1703,12 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C9">
-        <v>2010</v>
-      </c>
-      <c r="D9">
         <v>2014</v>
       </c>
       <c r="E9" t="b">
@@ -1717,10 +1717,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="C10">
         <v>2010</v>
@@ -1729,34 +1729,51 @@
         <v>2014</v>
       </c>
       <c r="E10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>2010</v>
       </c>
+      <c r="D11">
+        <v>2014</v>
+      </c>
       <c r="E11" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12">
+        <v>2010</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>2009</v>
       </c>
-      <c r="E12" t="b">
+      <c r="E13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1780,27 +1797,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update links and grant sorting
</commit_message>
<xml_diff>
--- a/cv-data.xlsx
+++ b/cv-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/websites/cv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5A27DD-B4C6-E643-8469-818DEE71AACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F08BAC3-4F48-4146-B3FE-799A3D114AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="26540" windowHeight="17040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="88">
   <si>
     <t>in_resume</t>
   </si>
@@ -200,9 +200,6 @@
     <t>sponsor</t>
   </si>
   <si>
-    <t>Innovations in Science Map, Assessment, and Reporting Technology (I-SMART)</t>
-  </si>
-  <si>
     <t>funding</t>
   </si>
   <si>
@@ -275,16 +272,22 @@
     <t>Honors Thesis: "[Dissociating Cognitive and Affective Empathy in Unipolar Depression](https://doi.org/10.31237/osf.io/m4xjf)"</t>
   </si>
   <si>
-    <t>Pathways for Instructionally Embedded Assessment (PIE)</t>
-  </si>
-  <si>
-    <t>Dynamic Learning Maps (DLM) Alternate Assessment System</t>
-  </si>
-  <si>
     <t>USED, Office of Elementary and Secondary Education, Office of School Support and Accountability</t>
   </si>
   <si>
     <t>Brooke Nash</t>
+  </si>
+  <si>
+    <t>[Dynamic Learning Maps (DLM) Alternate Assessment System](https://dynamiclearningmaps.org/)</t>
+  </si>
+  <si>
+    <t>[Pathways for Instructionally Embedded Assessment (PIE)](https://pie.atlas4learning.org/)</t>
+  </si>
+  <si>
+    <t>[Improving Software and Methods for Estimating and Evaluating Diagnostic Classification Models](https://measr.info)</t>
+  </si>
+  <si>
+    <t>[Innovations in Science Map, Assessment, and Reporting Technology (I-SMART)](https://ismart.works)</t>
   </si>
 </sst>
 </file>
@@ -1173,7 +1176,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J1" t="s">
         <v>0</v>
@@ -1196,10 +1199,10 @@
         <v>2018</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>13</v>
@@ -1225,16 +1228,16 @@
         <v>2014</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
@@ -1291,7 +1294,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K1" t="s">
         <v>0</v>
@@ -1299,7 +1302,7 @@
     </row>
     <row r="2" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -1311,19 +1314,19 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1343,7 +1346,7 @@
         <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1423,7 +1426,7 @@
         <v>29</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1435,8 +1438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B7310B-209B-5F48-96E7-648531B2B600}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1469,44 +1472,47 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" t="s">
         <v>59</v>
-      </c>
-      <c r="H1" t="s">
-        <v>60</v>
       </c>
       <c r="I1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>84</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>52</v>
       </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
       <c r="C3" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E3">
         <v>2022</v>
@@ -1518,10 +1524,10 @@
         <v>2500000</v>
       </c>
       <c r="H3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -1532,10 +1538,10 @@
         <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" t="s">
         <v>63</v>
-      </c>
-      <c r="D4" t="s">
-        <v>64</v>
       </c>
       <c r="E4">
         <v>2021</v>
@@ -1558,10 +1564,10 @@
         <v>56</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5">
         <v>2016</v>
@@ -1570,7 +1576,7 @@
         <v>2020</v>
       </c>
       <c r="H5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
@@ -1584,10 +1590,10 @@
         <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" t="s">
         <v>63</v>
-      </c>
-      <c r="D6" t="s">
-        <v>64</v>
       </c>
       <c r="E6">
         <v>2020</v>
@@ -1666,10 +1672,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3">
         <v>2023</v>
@@ -1680,10 +1686,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4">
         <v>2022</v>

</xml_diff>